<commit_message>
Filled columns with missed values
</commit_message>
<xml_diff>
--- a/COFCO.Forms/Files/TestTemp.xlsx
+++ b/COFCO.Forms/Files/TestTemp.xlsx
@@ -1,20 +1,96 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\VS Projects\ExcelWork\COFCO.Forms\Files\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8115"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211" refMode="R1C1"/>
+  <calcPr calcId="171027" refMode="R1C1"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="90">
+  <si>
+    <t>№ п/п</t>
+  </si>
+  <si>
+    <t>Продукт</t>
+  </si>
+  <si>
+    <t>Поставщик</t>
+  </si>
+  <si>
+    <t>Экспортер</t>
+  </si>
+  <si>
+    <t>Нерезидент</t>
+  </si>
+  <si>
+    <t>Договор экспортера</t>
+  </si>
+  <si>
+    <t>Контракт</t>
+  </si>
+  <si>
+    <t>Дата</t>
+  </si>
+  <si>
+    <t>Дата отправки</t>
+  </si>
+  <si>
+    <t>Порт</t>
+  </si>
+  <si>
+    <t>Пункт погрузки</t>
+  </si>
+  <si>
+    <t>Номер машини</t>
+  </si>
+  <si>
+    <t>ТТН</t>
+  </si>
+  <si>
+    <t>Перевозчик</t>
+  </si>
+  <si>
+    <t>Кількість</t>
+  </si>
+  <si>
+    <t>Вес по перевеске</t>
+  </si>
+  <si>
+    <t>Разница</t>
+  </si>
+  <si>
+    <t>Приход</t>
+  </si>
+  <si>
+    <t>Расход</t>
+  </si>
+  <si>
+    <t>Кон. Ост</t>
+  </si>
+  <si>
+    <t>По данным лаборатории</t>
+  </si>
+  <si>
+    <t>Вид операции</t>
+  </si>
   <si>
     <t>Кукурудза 3 класу кормові потреби</t>
   </si>
@@ -34,6 +110,9 @@
     <t>08.11.2016</t>
   </si>
   <si>
+    <t>14.11.2016 13:26:50</t>
+  </si>
+  <si>
     <t>Cofco Resources S.A.</t>
   </si>
   <si>
@@ -43,9 +122,6 @@
     <t>Приход (жд)</t>
   </si>
   <si>
-    <t>14.11.2016 13:26:50</t>
-  </si>
-  <si>
     <t>14.11.2016 13:29:33</t>
   </si>
   <si>
@@ -218,36 +294,12 @@
   </si>
   <si>
     <t>СА3645ВВ/СА1185ХР</t>
-  </si>
-  <si>
-    <t>Продукт</t>
-  </si>
-  <si>
-    <t>Поставщик</t>
-  </si>
-  <si>
-    <t>Контракт</t>
-  </si>
-  <si>
-    <t>Порт</t>
-  </si>
-  <si>
-    <t>Дата</t>
-  </si>
-  <si>
-    <t>Кількість</t>
-  </si>
-  <si>
-    <t>Номер машини</t>
-  </si>
-  <si>
-    <t>ТТН</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy;@"/>
     <numFmt numFmtId="165" formatCode="000000"/>
@@ -362,7 +414,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -385,44 +437,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -450,14 +502,31 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -485,6 +554,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -496,166 +582,142 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="35000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="80000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
               </a:schemeClr>
             </a:gs>
-            <a:gs pos="40000">
+            <a:gs pos="50000">
               <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -664,112 +726,115 @@
   <dimension ref="A1:W68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection sqref="A1:W68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="24.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>68</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>69</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3">
-        <v>548122</v>
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>70</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="I1" s="4">
-        <v>42688.547199074077</v>
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>71</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>75</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="O1" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="P1" s="5">
-        <v>66500</v>
-      </c>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="5">
-        <v>66500</v>
-      </c>
-      <c r="S1" s="6"/>
-      <c r="T1" s="5">
-        <v>66500</v>
-      </c>
-      <c r="U1" s="7">
-        <v>14.5</v>
-      </c>
-      <c r="V1" s="7">
-        <v>1.97</v>
+        <v>14</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>20</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="8"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>11246</v>
+      </c>
       <c r="B2" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D2" s="9" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E2" s="9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F2" s="10">
         <v>548122</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H2" s="9" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I2" s="9" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L2" s="10">
         <v>33192774</v>
@@ -798,37 +863,39 @@
       </c>
       <c r="W2" s="9"/>
     </row>
-    <row r="3" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+    <row r="3" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>11247</v>
+      </c>
       <c r="B3" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F3" s="3">
         <v>548122</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I3" s="4">
         <v>42688.560300925928</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L3" s="3">
         <v>33192774</v>
@@ -837,7 +904,7 @@
         <v>95378907</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O3" s="5">
         <v>66450</v>
@@ -862,40 +929,42 @@
         <v>1.96</v>
       </c>
       <c r="W3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>11248</v>
+      </c>
       <c r="B4" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F4" s="10">
         <v>548122</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L4" s="10">
         <v>33192774</v>
@@ -924,37 +993,39 @@
       </c>
       <c r="W4" s="9"/>
     </row>
-    <row r="5" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+    <row r="5" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>11250</v>
+      </c>
       <c r="B5" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F5" s="3">
         <v>548122</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I5" s="4">
         <v>42688.5621875</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L5" s="3">
         <v>33192774</v>
@@ -963,7 +1034,7 @@
         <v>95755401</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O5" s="5">
         <v>66900</v>
@@ -988,40 +1059,42 @@
         <v>2</v>
       </c>
       <c r="W5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>11252</v>
+      </c>
       <c r="B6" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F6" s="10">
         <v>548122</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I6" s="9" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K6" s="9" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L6" s="10">
         <v>33192774</v>
@@ -1050,37 +1123,39 @@
       </c>
       <c r="W6" s="9"/>
     </row>
-    <row r="7" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+    <row r="7" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>11254</v>
+      </c>
       <c r="B7" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F7" s="3">
         <v>548122</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="I7" s="4">
         <v>42688.562824074077</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L7" s="3">
         <v>33192774</v>
@@ -1089,7 +1164,7 @@
         <v>95667960</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O7" s="5">
         <v>67050</v>
@@ -1114,40 +1189,42 @@
         <v>1.98</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
+      <c r="A8" s="1">
+        <v>11256</v>
+      </c>
       <c r="B8" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F8" s="10">
         <v>555232</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I8" s="9" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L8" s="10">
         <v>44906204</v>
@@ -1177,36 +1254,38 @@
       <c r="W8" s="9"/>
     </row>
     <row r="9" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>11258</v>
+      </c>
       <c r="B9" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F9" s="3">
         <v>555232</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I9" s="4">
         <v>42688.564131944448</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L9" s="3">
         <v>44906204</v>
@@ -1215,7 +1294,7 @@
         <v>95988911</v>
       </c>
       <c r="N9" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O9" s="5">
         <v>65450</v>
@@ -1240,40 +1319,42 @@
         <v>1.95</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
+      <c r="A10" s="1">
+        <v>11260</v>
+      </c>
       <c r="B10" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F10" s="10">
         <v>555232</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I10" s="9" t="s">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K10" s="9" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L10" s="10">
         <v>44906204</v>
@@ -1303,36 +1384,38 @@
       <c r="W10" s="9"/>
     </row>
     <row r="11" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1">
+        <v>11246</v>
+      </c>
       <c r="B11" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F11" s="3">
         <v>555232</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I11" s="4">
         <v>42688.56490740741</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L11" s="3">
         <v>44906204</v>
@@ -1341,7 +1424,7 @@
         <v>95632105</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O11" s="5">
         <v>65400</v>
@@ -1366,40 +1449,42 @@
         <v>1.91</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="8">
+        <v>11247</v>
+      </c>
       <c r="B12" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F12" s="10">
         <v>555232</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I12" s="9" t="s">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K12" s="9" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L12" s="10">
         <v>44906204</v>
@@ -1429,36 +1514,38 @@
       <c r="W12" s="9"/>
     </row>
     <row r="13" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1">
+        <v>11248</v>
+      </c>
       <c r="B13" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F13" s="3">
         <v>555232</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I13" s="4">
         <v>42688.565671296295</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="L13" s="3">
         <v>44906204</v>
@@ -1467,7 +1554,7 @@
         <v>95969812</v>
       </c>
       <c r="N13" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O13" s="5">
         <v>62800</v>
@@ -1492,40 +1579,42 @@
         <v>1.88</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>11250</v>
+      </c>
       <c r="B14" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F14" s="3">
         <v>548122</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I14" s="4">
         <v>42688.646111111113</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L14" s="3">
         <v>33220757</v>
@@ -1534,7 +1623,7 @@
         <v>95799383</v>
       </c>
       <c r="N14" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O14" s="5">
         <v>67300</v>
@@ -1559,40 +1648,42 @@
         <v>1.97</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>11252</v>
+      </c>
       <c r="B15" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F15" s="3">
         <v>548122</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I15" s="4">
         <v>42688.646990740737</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L15" s="3">
         <v>33220757</v>
@@ -1601,7 +1692,7 @@
         <v>95644175</v>
       </c>
       <c r="N15" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O15" s="5">
         <v>67050</v>
@@ -1626,40 +1717,42 @@
         <v>1.95</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1">
+        <v>11254</v>
+      </c>
       <c r="B16" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F16" s="3">
         <v>550052</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I16" s="4">
         <v>42688.653333333335</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L16" s="3">
         <v>33223645</v>
@@ -1668,7 +1761,7 @@
         <v>95613774</v>
       </c>
       <c r="N16" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O16" s="5">
         <v>67250</v>
@@ -1693,40 +1786,42 @@
         <v>1.95</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1">
+        <v>11256</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F17" s="3">
         <v>550052</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I17" s="4">
         <v>42688.65415509259</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L17" s="3">
         <v>33223645</v>
@@ -1735,7 +1830,7 @@
         <v>95682779</v>
       </c>
       <c r="N17" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O17" s="5">
         <v>67500</v>
@@ -1760,40 +1855,42 @@
         <v>1.97</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
+      <c r="A18" s="1">
+        <v>11258</v>
+      </c>
       <c r="B18" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F18" s="3">
         <v>550052</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I18" s="4">
         <v>42688.654918981483</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L18" s="3">
         <v>33223645</v>
@@ -1802,7 +1899,7 @@
         <v>95681532</v>
       </c>
       <c r="N18" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O18" s="5">
         <v>67550</v>
@@ -1827,40 +1924,42 @@
         <v>1.95</v>
       </c>
       <c r="W18" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
+      <c r="A19" s="1">
+        <v>11260</v>
+      </c>
       <c r="B19" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F19" s="3">
         <v>550052</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I19" s="4">
         <v>42688.655578703707</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L19" s="3">
         <v>33223645</v>
@@ -1869,7 +1968,7 @@
         <v>95369609</v>
       </c>
       <c r="N19" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O19" s="5">
         <v>62600</v>
@@ -1894,40 +1993,42 @@
         <v>1.9</v>
       </c>
       <c r="W19" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
+      <c r="A20" s="1">
+        <v>11246</v>
+      </c>
       <c r="B20" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F20" s="3">
         <v>550052</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I20" s="4">
         <v>42688.656238425923</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L20" s="3">
         <v>33223645</v>
@@ -1936,7 +2037,7 @@
         <v>95353488</v>
       </c>
       <c r="N20" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O20" s="5">
         <v>67500</v>
@@ -1961,40 +2062,42 @@
         <v>1.99</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:23" ht="67.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="1"/>
+      <c r="A21" s="8">
+        <v>11247</v>
+      </c>
       <c r="B21" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F21" s="3">
         <v>550052</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I21" s="4">
         <v>42688.656909722224</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L21" s="3">
         <v>33223645</v>
@@ -2003,7 +2106,7 @@
         <v>95338414</v>
       </c>
       <c r="N21" s="2" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="O21" s="5">
         <v>67500</v>
@@ -2028,40 +2131,42 @@
         <v>1.98</v>
       </c>
       <c r="W21" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
+      <c r="A22" s="1">
+        <v>11248</v>
+      </c>
       <c r="B22" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="F22" s="3">
         <v>550052</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I22" s="4">
         <v>42688.657581018517</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="L22" s="3">
         <v>44901759</v>
@@ -2070,7 +2175,7 @@
         <v>95321725</v>
       </c>
       <c r="N22" s="2" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="O22" s="5">
         <v>63020</v>
@@ -2095,40 +2200,42 @@
         <v>1.92</v>
       </c>
       <c r="W22" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>11250</v>
+      </c>
       <c r="B23" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F23" s="3">
         <v>548122</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="I23" s="4">
         <v>42688.668854166666</v>
       </c>
       <c r="J23" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="L23" s="3">
         <v>33220757</v>
@@ -2137,7 +2244,7 @@
         <v>95392734</v>
       </c>
       <c r="N23" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O23" s="5">
         <v>66950</v>
@@ -2162,49 +2269,51 @@
         <v>1.95</v>
       </c>
       <c r="W23" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
+      <c r="A24" s="1">
+        <v>11252</v>
+      </c>
       <c r="B24" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>31</v>
+        <v>53</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I24" s="4">
         <v>42688.717013888891</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="L24" s="16">
         <v>44952</v>
       </c>
       <c r="M24" s="2" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="N24" s="2" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
       <c r="O24" s="5">
         <v>24600</v>
@@ -2229,40 +2338,42 @@
         <v>2</v>
       </c>
       <c r="W24" s="2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
+      <c r="A25" s="1">
+        <v>11254</v>
+      </c>
       <c r="B25" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H25" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="I25" s="4">
         <v>42688.942835648151</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="L25" s="3">
         <v>33226630</v>
@@ -2271,7 +2382,7 @@
         <v>95668646</v>
       </c>
       <c r="N25" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="O25" s="5">
         <v>67850</v>
@@ -2296,40 +2407,42 @@
         <v>1.95</v>
       </c>
       <c r="W25" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
+      <c r="A26" s="1">
+        <v>11256</v>
+      </c>
       <c r="B26" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="I26" s="4">
         <v>42688.94358796296</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K26" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="L26" s="3">
         <v>33226630</v>
@@ -2338,7 +2451,7 @@
         <v>95391579</v>
       </c>
       <c r="N26" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="O26" s="5">
         <v>64580</v>
@@ -2363,40 +2476,42 @@
         <v>1.94</v>
       </c>
       <c r="W26" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
+      <c r="A27" s="1">
+        <v>11258</v>
+      </c>
       <c r="B27" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C27" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H27" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="I27" s="4">
         <v>42688.944328703707</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="L27" s="3">
         <v>33226630</v>
@@ -2405,7 +2520,7 @@
         <v>95693578</v>
       </c>
       <c r="N27" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="O27" s="5">
         <v>67900</v>
@@ -2430,40 +2545,42 @@
         <v>1.96</v>
       </c>
       <c r="W27" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
+      <c r="A28" s="1">
+        <v>11260</v>
+      </c>
       <c r="B28" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I28" s="4">
         <v>42688.944976851853</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="L28" s="3">
         <v>33206053</v>
@@ -2472,7 +2589,7 @@
         <v>95756755</v>
       </c>
       <c r="N28" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="O28" s="5">
         <v>65300</v>
@@ -2497,40 +2614,42 @@
         <v>2</v>
       </c>
       <c r="W28" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
+      <c r="A29" s="1">
+        <v>11250</v>
+      </c>
       <c r="B29" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G29" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I29" s="4">
         <v>42688.945636574077</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="L29" s="3">
         <v>33206053</v>
@@ -2539,7 +2658,7 @@
         <v>95623823</v>
       </c>
       <c r="N29" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="O29" s="5">
         <v>66340</v>
@@ -2564,40 +2683,42 @@
         <v>2</v>
       </c>
       <c r="W29" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+      <c r="A30" s="1">
+        <v>11252</v>
+      </c>
       <c r="B30" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>38</v>
+        <v>60</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I30" s="4">
         <v>42688.946400462963</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="L30" s="3">
         <v>33206053</v>
@@ -2606,7 +2727,7 @@
         <v>95448932</v>
       </c>
       <c r="N30" s="2" t="s">
-        <v>41</v>
+        <v>63</v>
       </c>
       <c r="O30" s="5">
         <v>66920</v>
@@ -2631,40 +2752,42 @@
         <v>2</v>
       </c>
       <c r="W30" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
+      <c r="A31" s="1">
+        <v>11254</v>
+      </c>
       <c r="B31" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="F31" s="3">
         <v>553335</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="I31" s="4">
         <v>42688.949004629627</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="L31" s="3">
         <v>39305586</v>
@@ -2673,7 +2796,7 @@
         <v>95695367</v>
       </c>
       <c r="N31" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="O31" s="5">
         <v>62450</v>
@@ -2698,40 +2821,42 @@
         <v>2</v>
       </c>
       <c r="W31" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
+      <c r="A32" s="1">
+        <v>11256</v>
+      </c>
       <c r="B32" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="F32" s="3">
         <v>553335</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>48</v>
+        <v>70</v>
       </c>
       <c r="I32" s="4">
         <v>42688.949872685182</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>49</v>
+        <v>71</v>
       </c>
       <c r="L32" s="3">
         <v>39294046</v>
@@ -2740,7 +2865,7 @@
         <v>95523817</v>
       </c>
       <c r="N32" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="O32" s="5">
         <v>66000</v>
@@ -2765,40 +2890,42 @@
         <v>2</v>
       </c>
       <c r="W32" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
+      <c r="A33" s="1">
+        <v>11258</v>
+      </c>
       <c r="B33" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="F33" s="3">
         <v>553335</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
       <c r="I33" s="4">
         <v>42688.950243055559</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="L33" s="3">
         <v>39305586</v>
@@ -2807,7 +2934,7 @@
         <v>95359816</v>
       </c>
       <c r="N33" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="O33" s="5">
         <v>62200</v>
@@ -2832,40 +2959,42 @@
         <v>2</v>
       </c>
       <c r="W33" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>11260</v>
+      </c>
       <c r="B34" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F34" s="3">
         <v>555232</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I34" s="4">
         <v>42688.950335648151</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L34" s="3">
         <v>44936631</v>
@@ -2874,7 +3003,7 @@
         <v>95688255</v>
       </c>
       <c r="N34" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O34" s="5">
         <v>63000</v>
@@ -2899,40 +3028,42 @@
         <v>1.95</v>
       </c>
       <c r="W34" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
+      <c r="A35" s="1">
+        <v>11246</v>
+      </c>
       <c r="B35" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="F35" s="3">
         <v>553335</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="I35" s="4">
         <v>42688.950740740744</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="L35" s="3">
         <v>39314307</v>
@@ -2941,7 +3072,7 @@
         <v>95620662</v>
       </c>
       <c r="N35" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="O35" s="5">
         <v>63750</v>
@@ -2966,40 +3097,42 @@
         <v>2</v>
       </c>
       <c r="W35" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>11247</v>
+      </c>
       <c r="B36" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F36" s="3">
         <v>555232</v>
       </c>
       <c r="G36" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I36" s="4">
         <v>42688.950995370367</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L36" s="3">
         <v>44936631</v>
@@ -3008,7 +3141,7 @@
         <v>95686069</v>
       </c>
       <c r="N36" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O36" s="5">
         <v>63850</v>
@@ -3033,40 +3166,42 @@
         <v>1.97</v>
       </c>
       <c r="W36" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="37" spans="1:23" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="1"/>
+      <c r="A37" s="1">
+        <v>11248</v>
+      </c>
       <c r="B37" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="F37" s="3">
         <v>553335</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>52</v>
+        <v>74</v>
       </c>
       <c r="I37" s="4">
         <v>42688.95113425926</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>46</v>
+        <v>68</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="L37" s="3">
         <v>39314307</v>
@@ -3075,7 +3210,7 @@
         <v>95831533</v>
       </c>
       <c r="N37" s="2" t="s">
-        <v>42</v>
+        <v>64</v>
       </c>
       <c r="O37" s="5">
         <v>60800</v>
@@ -3100,40 +3235,42 @@
         <v>1.98</v>
       </c>
       <c r="W37" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="38" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>11250</v>
+      </c>
       <c r="B38" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F38" s="3">
         <v>555232</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I38" s="4">
         <v>42688.951504629629</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L38" s="3">
         <v>44936631</v>
@@ -3142,7 +3279,7 @@
         <v>95091963</v>
       </c>
       <c r="N38" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O38" s="5">
         <v>65100</v>
@@ -3167,40 +3304,42 @@
         <v>1.96</v>
       </c>
       <c r="W38" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>11252</v>
+      </c>
       <c r="B39" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F39" s="3">
         <v>555232</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I39" s="4">
         <v>42688.952002314814</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L39" s="3">
         <v>44936631</v>
@@ -3209,7 +3348,7 @@
         <v>95857066</v>
       </c>
       <c r="N39" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O39" s="5">
         <v>63500</v>
@@ -3234,40 +3373,42 @@
         <v>1.99</v>
       </c>
       <c r="W39" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A40" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="40" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>11254</v>
+      </c>
       <c r="B40" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F40" s="3">
         <v>555232</v>
       </c>
       <c r="G40" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I40" s="4">
         <v>42688.952499999999</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L40" s="3">
         <v>44936631</v>
@@ -3276,7 +3417,7 @@
         <v>95717039</v>
       </c>
       <c r="N40" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O40" s="5">
         <v>62250</v>
@@ -3301,40 +3442,42 @@
         <v>1.98</v>
       </c>
       <c r="W40" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A41" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>11256</v>
+      </c>
       <c r="B41" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F41" s="3">
         <v>555232</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I41" s="4">
         <v>42688.952916666669</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L41" s="3">
         <v>44936631</v>
@@ -3343,7 +3486,7 @@
         <v>95021150</v>
       </c>
       <c r="N41" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O41" s="5">
         <v>63900</v>
@@ -3368,40 +3511,42 @@
         <v>1.94</v>
       </c>
       <c r="W41" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>11258</v>
+      </c>
       <c r="B42" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F42" s="3">
         <v>555232</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I42" s="4">
         <v>42688.953344907408</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L42" s="3">
         <v>44936631</v>
@@ -3410,7 +3555,7 @@
         <v>95133211</v>
       </c>
       <c r="N42" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O42" s="5">
         <v>63800</v>
@@ -3435,40 +3580,42 @@
         <v>1.98</v>
       </c>
       <c r="W42" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>11260</v>
+      </c>
       <c r="B43" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F43" s="3">
         <v>555232</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I43" s="4">
         <v>42688.953750000001</v>
       </c>
       <c r="J43" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L43" s="3">
         <v>44936631</v>
@@ -3477,7 +3624,7 @@
         <v>95132916</v>
       </c>
       <c r="N43" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O43" s="5">
         <v>63100</v>
@@ -3502,40 +3649,42 @@
         <v>1.96</v>
       </c>
       <c r="W43" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A44" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>11246</v>
+      </c>
       <c r="B44" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F44" s="3">
         <v>555232</v>
       </c>
       <c r="G44" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I44" s="4">
         <v>42689.076331018521</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L44" s="3">
         <v>44936631</v>
@@ -3544,7 +3693,7 @@
         <v>95806949</v>
       </c>
       <c r="N44" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O44" s="5">
         <v>62450</v>
@@ -3569,40 +3718,42 @@
         <v>1.92</v>
       </c>
       <c r="W44" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="45" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A45" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>11247</v>
+      </c>
       <c r="B45" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F45" s="3">
         <v>555232</v>
       </c>
       <c r="G45" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H45" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I45" s="4">
         <v>42689.076805555553</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L45" s="3">
         <v>44936631</v>
@@ -3611,7 +3762,7 @@
         <v>95093506</v>
       </c>
       <c r="N45" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O45" s="5">
         <v>61600</v>
@@ -3636,40 +3787,42 @@
         <v>1.98</v>
       </c>
       <c r="W45" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A46" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>11248</v>
+      </c>
       <c r="B46" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F46" s="3">
         <v>555232</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H46" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I46" s="4">
         <v>42689.077199074076</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L46" s="3">
         <v>44936631</v>
@@ -3678,7 +3831,7 @@
         <v>95687828</v>
       </c>
       <c r="N46" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O46" s="5">
         <v>62550</v>
@@ -3703,40 +3856,42 @@
         <v>1.94</v>
       </c>
       <c r="W46" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="47" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A47" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>11250</v>
+      </c>
       <c r="B47" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F47" s="3">
         <v>555232</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I47" s="4">
         <v>42689.077604166669</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L47" s="3">
         <v>44936631</v>
@@ -3745,7 +3900,7 @@
         <v>95050902</v>
       </c>
       <c r="N47" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O47" s="5">
         <v>58700</v>
@@ -3770,40 +3925,42 @@
         <v>1.97</v>
       </c>
       <c r="W47" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="48" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A48" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="48" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>11252</v>
+      </c>
       <c r="B48" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G48" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H48" s="2" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="I48" s="4">
         <v>42689.078101851854</v>
       </c>
       <c r="J48" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K48" s="2" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="L48" s="3">
         <v>42256081</v>
@@ -3812,7 +3969,7 @@
         <v>95644654</v>
       </c>
       <c r="N48" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O48" s="5">
         <v>67100</v>
@@ -3837,40 +3994,42 @@
         <v>1.95</v>
       </c>
       <c r="W48" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A49" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="49" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>11254</v>
+      </c>
       <c r="B49" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>53</v>
+        <v>75</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>54</v>
+        <v>76</v>
       </c>
       <c r="I49" s="4">
         <v>42689.07849537037</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="L49" s="3">
         <v>42256081</v>
@@ -3879,7 +4038,7 @@
         <v>95348827</v>
       </c>
       <c r="N49" s="2" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="O49" s="5">
         <v>66700</v>
@@ -3904,40 +4063,42 @@
         <v>1.93</v>
       </c>
       <c r="W49" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="50" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1">
+        <v>11256</v>
+      </c>
       <c r="B50" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H50" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I50" s="4">
         <v>42689.078935185185</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K50" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="L50" s="3">
         <v>44903466</v>
@@ -3946,7 +4107,7 @@
         <v>95523627</v>
       </c>
       <c r="N50" s="2" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="O50" s="5">
         <v>66800</v>
@@ -3971,40 +4132,42 @@
         <v>1.93</v>
       </c>
       <c r="W50" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A51" s="1"/>
+      <c r="A51" s="1">
+        <v>11258</v>
+      </c>
       <c r="B51" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H51" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I51" s="4">
         <v>42689.079328703701</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K51" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="L51" s="3">
         <v>44903466</v>
@@ -4013,7 +4176,7 @@
         <v>95799771</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="O51" s="5">
         <v>66500</v>
@@ -4038,40 +4201,42 @@
         <v>1.92</v>
       </c>
       <c r="W51" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="52" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A52" s="1"/>
+      <c r="A52" s="1">
+        <v>11260</v>
+      </c>
       <c r="B52" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H52" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I52" s="4">
         <v>42689.079907407409</v>
       </c>
       <c r="J52" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K52" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="L52" s="3">
         <v>44903466</v>
@@ -4080,7 +4245,7 @@
         <v>95799268</v>
       </c>
       <c r="N52" s="2" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="O52" s="5">
         <v>67000</v>
@@ -4105,40 +4270,42 @@
         <v>1.95</v>
       </c>
       <c r="W52" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A53" s="1"/>
+      <c r="A53" s="1">
+        <v>11260</v>
+      </c>
       <c r="B53" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>56</v>
+        <v>78</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H53" s="2" t="s">
-        <v>29</v>
+        <v>51</v>
       </c>
       <c r="I53" s="4">
         <v>42689.080300925925</v>
       </c>
       <c r="J53" s="2" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="K53" s="2" t="s">
-        <v>57</v>
+        <v>79</v>
       </c>
       <c r="L53" s="3">
         <v>44903466</v>
@@ -4147,7 +4314,7 @@
         <v>95829677</v>
       </c>
       <c r="N53" s="2" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
       <c r="O53" s="5">
         <v>66450</v>
@@ -4172,44 +4339,46 @@
         <v>1.96</v>
       </c>
       <c r="W53" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
     <row r="54" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A54" s="8"/>
+      <c r="A54" s="1">
+        <v>11246</v>
+      </c>
       <c r="B54" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D54" s="9" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E54" s="9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F54" s="9"/>
       <c r="G54" s="9" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H54" s="9" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I54" s="9" t="s">
-        <v>61</v>
+        <v>83</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K54" s="9" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="L54" s="10">
         <v>2041</v>
       </c>
       <c r="M54" s="9" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="N54" s="9"/>
       <c r="O54" s="11">
@@ -4233,45 +4402,47 @@
       <c r="W54" s="9"/>
     </row>
     <row r="55" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="1"/>
+      <c r="A55" s="8">
+        <v>11247</v>
+      </c>
       <c r="B55" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H55" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I55" s="4">
         <v>42689.12804398148</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K55" s="2" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="L55" s="3">
         <v>2041</v>
       </c>
       <c r="M55" s="2" t="s">
-        <v>63</v>
+        <v>85</v>
       </c>
       <c r="N55" s="2" t="s">
-        <v>64</v>
+        <v>86</v>
       </c>
       <c r="O55" s="5">
         <v>20980</v>
@@ -4296,44 +4467,46 @@
         <v>1.94</v>
       </c>
       <c r="W55" s="2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="56" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
+      <c r="A56" s="1">
+        <v>11248</v>
+      </c>
       <c r="B56" s="9" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D56" s="9" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E56" s="9" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F56" s="9"/>
       <c r="G56" s="9" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H56" s="9" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I56" s="9" t="s">
-        <v>65</v>
+        <v>87</v>
       </c>
       <c r="J56" s="9" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K56" s="9" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="L56" s="10">
         <v>2043</v>
       </c>
       <c r="M56" s="9" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="N56" s="9"/>
       <c r="O56" s="11">
@@ -4357,45 +4530,47 @@
       <c r="W56" s="9"/>
     </row>
     <row r="57" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A57" s="1"/>
+      <c r="A57" s="1">
+        <v>11250</v>
+      </c>
       <c r="B57" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H57" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I57" s="4">
         <v>42689.13181712963</v>
       </c>
       <c r="J57" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K57" s="2" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="L57" s="3">
         <v>2043</v>
       </c>
       <c r="M57" s="2" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="N57" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="O57" s="5">
         <v>21880</v>
@@ -4420,49 +4595,51 @@
         <v>1.88</v>
       </c>
       <c r="W57" s="2" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
     </row>
     <row r="58" spans="1:23" ht="56.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="1"/>
+      <c r="A58" s="1">
+        <v>11252</v>
+      </c>
       <c r="B58" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>3</v>
+        <v>25</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>32</v>
+        <v>54</v>
       </c>
       <c r="H58" s="2" t="s">
-        <v>60</v>
+        <v>82</v>
       </c>
       <c r="I58" s="4">
         <v>42689.136990740742</v>
       </c>
       <c r="J58" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K58" s="2" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="L58" s="3">
         <v>2042</v>
       </c>
       <c r="M58" s="2" t="s">
-        <v>67</v>
+        <v>89</v>
       </c>
       <c r="N58" s="2" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="O58" s="5">
         <v>20270</v>
@@ -4487,40 +4664,42 @@
         <v>2</v>
       </c>
       <c r="W58" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="59" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="1"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>11254</v>
+      </c>
       <c r="B59" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F59" s="3">
         <v>555232</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H59" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I59" s="4">
         <v>42689.138645833336</v>
       </c>
       <c r="J59" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K59" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L59" s="3">
         <v>44936631</v>
@@ -4529,7 +4708,7 @@
         <v>95460028</v>
       </c>
       <c r="N59" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O59" s="5">
         <v>63050</v>
@@ -4554,40 +4733,42 @@
         <v>1.96</v>
       </c>
       <c r="W59" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="60" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A60" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>11256</v>
+      </c>
       <c r="B60" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F60" s="3">
         <v>555232</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H60" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I60" s="4">
         <v>42689.13921296296</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K60" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L60" s="3">
         <v>44936631</v>
@@ -4596,7 +4777,7 @@
         <v>95689089</v>
       </c>
       <c r="N60" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O60" s="5">
         <v>63350</v>
@@ -4619,40 +4800,42 @@
         <v>1.91</v>
       </c>
       <c r="W60" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="61" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A61" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="61" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>11258</v>
+      </c>
       <c r="B61" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F61" s="3">
         <v>555232</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I61" s="4">
         <v>42689.139803240738</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K61" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L61" s="3">
         <v>44936631</v>
@@ -4661,7 +4844,7 @@
         <v>95069167</v>
       </c>
       <c r="N61" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O61" s="5">
         <v>64350</v>
@@ -4686,40 +4869,42 @@
         <v>1.93</v>
       </c>
       <c r="W61" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="62" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A62" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="62" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>11260</v>
+      </c>
       <c r="B62" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F62" s="3">
         <v>555232</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H62" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I62" s="4">
         <v>42689.1405787037</v>
       </c>
       <c r="J62" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K62" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L62" s="3">
         <v>44937852</v>
@@ -4728,7 +4913,7 @@
         <v>95129334</v>
       </c>
       <c r="N62" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O62" s="5">
         <v>64200</v>
@@ -4753,40 +4938,42 @@
         <v>1.9</v>
       </c>
       <c r="W62" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="63" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A63" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="63" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>11246</v>
+      </c>
       <c r="B63" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F63" s="3">
         <v>555232</v>
       </c>
       <c r="G63" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H63" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I63" s="4">
         <v>42689.141134259262</v>
       </c>
       <c r="J63" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K63" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L63" s="3">
         <v>44937852</v>
@@ -4795,7 +4982,7 @@
         <v>95129409</v>
       </c>
       <c r="N63" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O63" s="5">
         <v>65000</v>
@@ -4818,40 +5005,42 @@
         <v>1.95</v>
       </c>
       <c r="W63" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A64" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="64" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="8">
+        <v>11247</v>
+      </c>
       <c r="B64" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F64" s="3">
         <v>555232</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H64" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I64" s="4">
         <v>42689.141597222224</v>
       </c>
       <c r="J64" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K64" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L64" s="3">
         <v>44937852</v>
@@ -4860,7 +5049,7 @@
         <v>95139119</v>
       </c>
       <c r="N64" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O64" s="5">
         <v>63100</v>
@@ -4885,40 +5074,42 @@
         <v>1.98</v>
       </c>
       <c r="W64" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="65" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A65" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="1">
+        <v>11248</v>
+      </c>
       <c r="B65" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F65" s="3">
         <v>555232</v>
       </c>
       <c r="G65" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H65" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I65" s="4">
         <v>42689.142754629633</v>
       </c>
       <c r="J65" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K65" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L65" s="3">
         <v>44937852</v>
@@ -4927,7 +5118,7 @@
         <v>95421103</v>
       </c>
       <c r="N65" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O65" s="5">
         <v>63300</v>
@@ -4952,40 +5143,42 @@
         <v>1.98</v>
       </c>
       <c r="W65" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="66" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A66" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="66" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A66" s="1">
+        <v>11250</v>
+      </c>
       <c r="B66" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F66" s="3">
         <v>555232</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H66" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I66" s="4">
         <v>42689.143263888887</v>
       </c>
       <c r="J66" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K66" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L66" s="3">
         <v>44937852</v>
@@ -4994,7 +5187,7 @@
         <v>95856969</v>
       </c>
       <c r="N66" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O66" s="5">
         <v>63100</v>
@@ -5019,40 +5212,42 @@
         <v>1.95</v>
       </c>
       <c r="W66" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="67" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="67" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A67" s="1">
+        <v>11252</v>
+      </c>
       <c r="B67" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F67" s="3">
         <v>555232</v>
       </c>
       <c r="G67" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H67" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I67" s="4">
         <v>42689.143807870372</v>
       </c>
       <c r="J67" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K67" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L67" s="3">
         <v>44937852</v>
@@ -5061,7 +5256,7 @@
         <v>95807053</v>
       </c>
       <c r="N67" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O67" s="5">
         <v>63500</v>
@@ -5086,40 +5281,42 @@
         <v>1.98</v>
       </c>
       <c r="W67" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:23" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="1"/>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+      <c r="A68" s="1">
+        <v>11254</v>
+      </c>
       <c r="B68" s="2" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
       <c r="F68" s="3">
         <v>555232</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="H68" s="2" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="I68" s="4">
         <v>42689.144432870373</v>
       </c>
       <c r="J68" s="2" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="K68" s="2" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
       <c r="L68" s="3">
         <v>44937852</v>
@@ -5128,7 +5325,7 @@
         <v>95657722</v>
       </c>
       <c r="N68" s="2" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="O68" s="5">
         <v>63250</v>
@@ -5153,7 +5350,7 @@
         <v>1.93</v>
       </c>
       <c r="W68" s="2" t="s">
-        <v>8</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>